<commit_message>
add test for parent with quote
</commit_message>
<xml_diff>
--- a/data/samples/ParentSamples.xlsx
+++ b/data/samples/ParentSamples.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A13215-E77A-3448-BE62-9CAB723014E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00CABB7-C353-0D43-8EFA-20F70D1E973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{2704F8E4-3691-EB47-AEE9-813C8905D274}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>MaterialInputs/Parent_SampleType</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>parent01,#parent04</t>
+  </si>
+  <si>
+    <t>"parent05</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578DAFC4-1960-8043-AF60-4BEE8DEE8C0D}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,6 +450,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix deriving from parent sample containing comma
</commit_message>
<xml_diff>
--- a/data/samples/ParentSamples.xlsx
+++ b/data/samples/ParentSamples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00CABB7-C353-0D43-8EFA-20F70D1E973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EFC60C-D801-0D4D-8021-58EA17FAC408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{2704F8E4-3691-EB47-AEE9-813C8905D274}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MaterialInputs/Parent_SampleType</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>"parent05</t>
+  </si>
+  <si>
+    <t>"parent,06"</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578DAFC4-1960-8043-AF60-4BEE8DEE8C0D}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,6 +458,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix deriving from parent sample containing comma (#2020)
</commit_message>
<xml_diff>
--- a/data/samples/ParentSamples.xlsx
+++ b/data/samples/ParentSamples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00CABB7-C353-0D43-8EFA-20F70D1E973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EFC60C-D801-0D4D-8021-58EA17FAC408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{2704F8E4-3691-EB47-AEE9-813C8905D274}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MaterialInputs/Parent_SampleType</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>"parent05</t>
+  </si>
+  <si>
+    <t>"parent,06"</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578DAFC4-1960-8043-AF60-4BEE8DEE8C0D}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,6 +458,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add selenium tests for Issue 51056
</commit_message>
<xml_diff>
--- a/data/samples/ParentSamples.xlsx
+++ b/data/samples/ParentSamples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EFC60C-D801-0D4D-8021-58EA17FAC408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054D31F9-DF28-8B4D-9244-1E49BAE5786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{2704F8E4-3691-EB47-AEE9-813C8905D274}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MaterialInputs/Parent_SampleType</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>"parent,06"</t>
+  </si>
+  <si>
+    <t>"parent07, "parent05</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578DAFC4-1960-8043-AF60-4BEE8DEE8C0D}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,6 +466,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add selenium tests for Issue 51056 (#2085)
</commit_message>
<xml_diff>
--- a/data/samples/ParentSamples.xlsx
+++ b/data/samples/ParentSamples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xingyang/dev/trunk/server/testAutomation/data/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EFC60C-D801-0D4D-8021-58EA17FAC408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054D31F9-DF28-8B4D-9244-1E49BAE5786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3200" windowWidth="28040" windowHeight="17440" xr2:uid="{2704F8E4-3691-EB47-AEE9-813C8905D274}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MaterialInputs/Parent_SampleType</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>"parent,06"</t>
+  </si>
+  <si>
+    <t>"parent07, "parent05</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578DAFC4-1960-8043-AF60-4BEE8DEE8C0D}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -463,6 +466,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>